<commit_message>
more work on PrOD combination tables.
</commit_message>
<xml_diff>
--- a/tabular/contributed/190612 DSV TABLE.xlsx
+++ b/tabular/contributed/190612 DSV TABLE.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="43020" windowHeight="26380"/>
+    <workbookView xWindow="6820" yWindow="460" windowWidth="43020" windowHeight="26380"/>
   </bookViews>
   <sheets>
     <sheet name="DSV" sheetId="3" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="101">
   <si>
     <t>gene</t>
   </si>
@@ -131,9 +131,6 @@
     <t>NS5B</t>
   </si>
   <si>
-    <t>S556G</t>
-  </si>
-  <si>
     <t>PEARL III, IV</t>
   </si>
   <si>
@@ -149,45 +146,21 @@
     <t>23</t>
   </si>
   <si>
-    <t>M414T+S556G</t>
-  </si>
-  <si>
-    <t>C316Y+S556G</t>
-  </si>
-  <si>
-    <t>G554S+S556G</t>
-  </si>
-  <si>
-    <t>D559G</t>
-  </si>
-  <si>
-    <t>A553T</t>
-  </si>
-  <si>
     <t>M414I</t>
   </si>
   <si>
-    <t>G558R</t>
-  </si>
-  <si>
     <t>non cirrhotic; TN and TE</t>
   </si>
   <si>
     <t>AVIATOR</t>
   </si>
   <si>
-    <t>C316N+S556G</t>
-  </si>
-  <si>
     <t xml:space="preserve">non cirrhotic; TN  </t>
   </si>
   <si>
     <t>GARNET</t>
   </si>
   <si>
-    <t>S556R</t>
-  </si>
-  <si>
     <t>TN &amp; TE; noncirrhotic and cirrhotic</t>
   </si>
   <si>
@@ -212,12 +185,6 @@
     <t xml:space="preserve">Sapphire II </t>
   </si>
   <si>
-    <t>159F+C316N</t>
-  </si>
-  <si>
-    <t>C316N +S556G</t>
-  </si>
-  <si>
     <t>TE, non cirrhotic</t>
   </si>
   <si>
@@ -230,42 +197,15 @@
     <t>real world, retrospective</t>
   </si>
   <si>
-    <t>C316N</t>
-  </si>
-  <si>
     <t>2-20</t>
   </si>
   <si>
     <t>10-20</t>
   </si>
   <si>
-    <t xml:space="preserve">C316Y </t>
-  </si>
-  <si>
-    <t xml:space="preserve">M414T </t>
-  </si>
-  <si>
-    <t>Y448C</t>
-  </si>
-  <si>
-    <t>Y448H</t>
-  </si>
-  <si>
-    <t>C316Y</t>
-  </si>
-  <si>
-    <t>S368T</t>
-  </si>
-  <si>
     <t>11</t>
   </si>
   <si>
-    <t>N411S</t>
-  </si>
-  <si>
-    <t>M414T</t>
-  </si>
-  <si>
     <t>1472</t>
   </si>
   <si>
@@ -296,52 +236,103 @@
     <t>414</t>
   </si>
   <si>
-    <t>A553V</t>
-  </si>
-  <si>
     <t>120</t>
   </si>
   <si>
-    <t>A395G</t>
-  </si>
-  <si>
-    <t>N444K</t>
-  </si>
-  <si>
-    <t>S556N</t>
-  </si>
-  <si>
-    <t>S565F</t>
-  </si>
-  <si>
     <t>17</t>
   </si>
   <si>
-    <t>C445F</t>
-  </si>
-  <si>
     <t>16</t>
   </si>
   <si>
-    <t>C451S</t>
-  </si>
-  <si>
-    <t>I585V</t>
-  </si>
-  <si>
-    <t>P495A</t>
-  </si>
-  <si>
     <t>2.4</t>
   </si>
   <si>
     <t>NK</t>
   </si>
   <si>
-    <t>C316Y+M414I</t>
-  </si>
-  <si>
     <t>cirrhosis</t>
+  </si>
+  <si>
+    <t>556G</t>
+  </si>
+  <si>
+    <t>414T+556G</t>
+  </si>
+  <si>
+    <t>316Y+556G</t>
+  </si>
+  <si>
+    <t>554S+556G</t>
+  </si>
+  <si>
+    <t>559G</t>
+  </si>
+  <si>
+    <t>553T</t>
+  </si>
+  <si>
+    <t>414I</t>
+  </si>
+  <si>
+    <t>558R</t>
+  </si>
+  <si>
+    <t>316N+556G</t>
+  </si>
+  <si>
+    <t>556R</t>
+  </si>
+  <si>
+    <t>316N</t>
+  </si>
+  <si>
+    <t>316Y</t>
+  </si>
+  <si>
+    <t>414T</t>
+  </si>
+  <si>
+    <t>448C</t>
+  </si>
+  <si>
+    <t>448H</t>
+  </si>
+  <si>
+    <t>368T</t>
+  </si>
+  <si>
+    <t>411S</t>
+  </si>
+  <si>
+    <t>553V</t>
+  </si>
+  <si>
+    <t>395G</t>
+  </si>
+  <si>
+    <t>444K</t>
+  </si>
+  <si>
+    <t>556N</t>
+  </si>
+  <si>
+    <t>565F</t>
+  </si>
+  <si>
+    <t>445F</t>
+  </si>
+  <si>
+    <t>451S</t>
+  </si>
+  <si>
+    <t>585V</t>
+  </si>
+  <si>
+    <t>495A</t>
+  </si>
+  <si>
+    <t>316Y+414I</t>
   </si>
 </sst>
 </file>
@@ -769,17 +760,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="168" zoomScaleNormal="168" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="168" zoomScaleNormal="168" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="I1" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="L22" sqref="L22"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.5" style="3" customWidth="1"/>
-    <col min="2" max="2" width="8.83203125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="24.1640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" style="3" customWidth="1"/>
     <col min="4" max="5" width="8.83203125" style="3"/>
     <col min="6" max="6" width="12.83203125" style="3" customWidth="1"/>
     <col min="7" max="7" width="8.83203125" style="3" customWidth="1"/>
@@ -799,10 +790,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>2</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>3</v>
@@ -849,10 +840,10 @@
         <v>32</v>
       </c>
       <c r="B2" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>22</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>60</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>17</v>
@@ -891,10 +882,10 @@
         <v>32</v>
       </c>
       <c r="B3" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>22</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>33</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>18</v>
@@ -933,10 +924,10 @@
         <v>32</v>
       </c>
       <c r="B4" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>16</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>33</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>18</v>
@@ -955,10 +946,10 @@
       </c>
       <c r="I4" s="9"/>
       <c r="J4" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="K4" s="8" t="s">
         <v>34</v>
-      </c>
-      <c r="K4" s="8" t="s">
-        <v>35</v>
       </c>
       <c r="L4" s="8" t="s">
         <v>21</v>
@@ -975,10 +966,10 @@
         <v>32</v>
       </c>
       <c r="B5" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>16</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>33</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>17</v>
@@ -997,13 +988,13 @@
       </c>
       <c r="I5" s="9"/>
       <c r="J5" s="8" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="K5" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L5" s="8" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="M5" s="8"/>
       <c r="N5" s="2"/>
@@ -1017,10 +1008,10 @@
         <v>32</v>
       </c>
       <c r="B6" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C6" s="8" t="s">
         <v>16</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>39</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>18</v>
@@ -1039,13 +1030,13 @@
       </c>
       <c r="I6" s="9"/>
       <c r="J6" s="8" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="K6" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="M6" s="8"/>
       <c r="N6" s="2"/>
@@ -1059,10 +1050,10 @@
         <v>32</v>
       </c>
       <c r="B7" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>16</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>40</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>17</v>
@@ -1081,13 +1072,13 @@
       </c>
       <c r="I7" s="9"/>
       <c r="J7" s="8" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="K7" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L7" s="8" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="M7" s="8"/>
       <c r="N7" s="2"/>
@@ -1101,10 +1092,10 @@
         <v>32</v>
       </c>
       <c r="B8" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>16</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>41</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>18</v>
@@ -1123,13 +1114,13 @@
       </c>
       <c r="I8" s="9"/>
       <c r="J8" s="8" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="K8" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L8" s="8" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="M8" s="8"/>
       <c r="N8" s="2"/>
@@ -1143,10 +1134,10 @@
         <v>32</v>
       </c>
       <c r="B9" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C9" s="8" t="s">
         <v>16</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>42</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>18</v>
@@ -1165,13 +1156,13 @@
       </c>
       <c r="I9" s="9"/>
       <c r="J9" s="8" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="K9" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="M9" s="8"/>
       <c r="N9" s="2"/>
@@ -1185,10 +1176,10 @@
         <v>32</v>
       </c>
       <c r="B10" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C10" s="8" t="s">
         <v>16</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>43</v>
       </c>
       <c r="D10" s="8" t="s">
         <v>18</v>
@@ -1207,13 +1198,13 @@
       </c>
       <c r="I10" s="9"/>
       <c r="J10" s="8" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="K10" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L10" s="8" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="M10" s="8"/>
       <c r="N10" s="2"/>
@@ -1227,10 +1218,10 @@
         <v>32</v>
       </c>
       <c r="B11" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C11" s="8" t="s">
         <v>16</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>44</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>17</v>
@@ -1249,13 +1240,13 @@
       </c>
       <c r="I11" s="9"/>
       <c r="J11" s="8" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="K11" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L11" s="8" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="M11" s="8"/>
       <c r="N11" s="2"/>
@@ -1269,10 +1260,10 @@
         <v>32</v>
       </c>
       <c r="B12" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C12" s="8" t="s">
         <v>16</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>45</v>
       </c>
       <c r="D12" s="8" t="s">
         <v>18</v>
@@ -1281,7 +1272,7 @@
         <v>17</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="G12" s="8" t="s">
         <v>30</v>
@@ -1291,13 +1282,13 @@
       </c>
       <c r="I12" s="9"/>
       <c r="J12" s="8" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="K12" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L12" s="8" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="M12" s="8"/>
       <c r="N12" s="2"/>
@@ -1311,10 +1302,10 @@
         <v>32</v>
       </c>
       <c r="B13" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C13" s="8" t="s">
         <v>22</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>48</v>
       </c>
       <c r="D13" s="8" t="s">
         <v>17</v>
@@ -1333,13 +1324,13 @@
       </c>
       <c r="I13" s="9"/>
       <c r="J13" s="8" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="K13" s="8" t="s">
         <v>31</v>
       </c>
       <c r="L13" s="8" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="M13" s="8"/>
       <c r="N13" s="2"/>
@@ -1353,10 +1344,10 @@
         <v>32</v>
       </c>
       <c r="B14" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C14" s="8" t="s">
         <v>16</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>51</v>
       </c>
       <c r="D14" s="8" t="s">
         <v>17</v>
@@ -1375,20 +1366,20 @@
       </c>
       <c r="I14" s="9"/>
       <c r="J14" s="8" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="K14" s="9" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="L14" s="8" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="M14" s="8"/>
       <c r="N14" s="8" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="O14" s="8" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="P14" s="8"/>
     </row>
@@ -1397,10 +1388,10 @@
         <v>32</v>
       </c>
       <c r="B15" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="C15" s="12" t="s">
         <v>16</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>33</v>
       </c>
       <c r="D15" s="12" t="s">
         <v>18</v>
@@ -1417,13 +1408,13 @@
       </c>
       <c r="I15" s="9"/>
       <c r="J15" s="12" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="K15" s="8" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="L15" s="8" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="M15" s="2"/>
       <c r="N15" s="8"/>
@@ -1437,10 +1428,10 @@
         <v>32</v>
       </c>
       <c r="B16" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C16" s="12" t="s">
         <v>22</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>61</v>
       </c>
       <c r="D16" s="12" t="s">
         <v>18</v>
@@ -1457,13 +1448,13 @@
       </c>
       <c r="I16" s="9"/>
       <c r="J16" s="12" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="K16" s="8" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="L16" s="8" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="M16" s="2"/>
       <c r="N16" s="8"/>
@@ -1477,10 +1468,10 @@
         <v>32</v>
       </c>
       <c r="B17" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="C17" s="12" t="s">
         <v>16</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>33</v>
       </c>
       <c r="D17" s="8" t="s">
         <v>18</v>
@@ -1497,13 +1488,13 @@
       </c>
       <c r="I17" s="9"/>
       <c r="J17" s="8" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="K17" s="8" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="L17" s="8" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="M17" s="2"/>
       <c r="N17" s="8"/>
@@ -1517,10 +1508,10 @@
         <v>32</v>
       </c>
       <c r="B18" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="C18" s="12" t="s">
         <v>16</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>33</v>
       </c>
       <c r="D18" s="12" t="s">
         <v>18</v>
@@ -1537,7 +1528,7 @@
       </c>
       <c r="I18" s="9"/>
       <c r="J18" s="8" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="K18" s="8" t="s">
         <v>31</v>
@@ -1555,10 +1546,10 @@
         <v>32</v>
       </c>
       <c r="B19" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="C19" s="12" t="s">
         <v>22</v>
-      </c>
-      <c r="C19" s="12" t="s">
-        <v>66</v>
       </c>
       <c r="D19" s="12" t="s">
         <v>18</v>
@@ -1589,10 +1580,10 @@
         <v>32</v>
       </c>
       <c r="B20" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="C20" s="12" t="s">
         <v>22</v>
-      </c>
-      <c r="C20" s="12" t="s">
-        <v>66</v>
       </c>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
@@ -1604,7 +1595,7 @@
         <v>25</v>
       </c>
       <c r="I20" s="9" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="J20" s="8"/>
       <c r="K20" s="8"/>
@@ -1621,10 +1612,10 @@
         <v>32</v>
       </c>
       <c r="B21" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="C21" s="12" t="s">
         <v>22</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>33</v>
       </c>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
@@ -1636,7 +1627,7 @@
         <v>25</v>
       </c>
       <c r="I21" s="9" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="J21" s="8"/>
       <c r="K21" s="8"/>
@@ -1653,10 +1644,10 @@
         <v>32</v>
       </c>
       <c r="B22" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="C22" s="12" t="s">
         <v>22</v>
-      </c>
-      <c r="C22" s="12" t="s">
-        <v>33</v>
       </c>
       <c r="D22" s="12" t="s">
         <v>18</v>
@@ -1673,7 +1664,7 @@
       </c>
       <c r="I22" s="9"/>
       <c r="J22" s="8" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="K22" s="8" t="s">
         <v>31</v>
@@ -1691,10 +1682,10 @@
         <v>32</v>
       </c>
       <c r="B23" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="C23" s="12" t="s">
         <v>16</v>
-      </c>
-      <c r="C23" s="12" t="s">
-        <v>69</v>
       </c>
       <c r="D23" s="8"/>
       <c r="E23" s="8"/>
@@ -1706,7 +1697,7 @@
         <v>25</v>
       </c>
       <c r="I23" s="9" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="J23" s="8"/>
       <c r="K23" s="8"/>
@@ -1723,10 +1714,10 @@
         <v>32</v>
       </c>
       <c r="B24" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="C24" s="12" t="s">
         <v>16</v>
-      </c>
-      <c r="C24" s="12" t="s">
-        <v>70</v>
       </c>
       <c r="D24" s="8"/>
       <c r="E24" s="8"/>
@@ -1738,7 +1729,7 @@
         <v>25</v>
       </c>
       <c r="I24" s="9" t="s">
-        <v>79</v>
+        <v>59</v>
       </c>
       <c r="J24" s="8"/>
       <c r="K24" s="8"/>
@@ -1755,10 +1746,10 @@
         <v>32</v>
       </c>
       <c r="B25" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="C25" s="12" t="s">
         <v>16</v>
-      </c>
-      <c r="C25" s="12" t="s">
-        <v>71</v>
       </c>
       <c r="D25" s="8"/>
       <c r="E25" s="8"/>
@@ -1770,7 +1761,7 @@
         <v>25</v>
       </c>
       <c r="I25" s="9" t="s">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="J25" s="8"/>
       <c r="K25" s="8"/>
@@ -1787,10 +1778,10 @@
         <v>32</v>
       </c>
       <c r="B26" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="C26" s="12" t="s">
         <v>16</v>
-      </c>
-      <c r="C26" s="12" t="s">
-        <v>72</v>
       </c>
       <c r="D26" s="8"/>
       <c r="E26" s="8"/>
@@ -1802,7 +1793,7 @@
         <v>25</v>
       </c>
       <c r="I26" s="9" t="s">
-        <v>81</v>
+        <v>61</v>
       </c>
       <c r="J26" s="8"/>
       <c r="K26" s="8"/>
@@ -1819,10 +1810,10 @@
         <v>32</v>
       </c>
       <c r="B27" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="C27" s="12" t="s">
         <v>16</v>
-      </c>
-      <c r="C27" s="12" t="s">
-        <v>33</v>
       </c>
       <c r="D27" s="8"/>
       <c r="E27" s="8"/>
@@ -1834,7 +1825,7 @@
         <v>25</v>
       </c>
       <c r="I27" s="9" t="s">
-        <v>82</v>
+        <v>62</v>
       </c>
       <c r="J27" s="8"/>
       <c r="K27" s="8"/>
@@ -1851,10 +1842,10 @@
         <v>32</v>
       </c>
       <c r="B28" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C28" s="8" t="s">
         <v>22</v>
-      </c>
-      <c r="C28" s="12" t="s">
-        <v>66</v>
       </c>
       <c r="D28" s="8"/>
       <c r="E28" s="8"/>
@@ -1866,7 +1857,7 @@
         <v>25</v>
       </c>
       <c r="I28" s="9" t="s">
-        <v>83</v>
+        <v>63</v>
       </c>
       <c r="J28" s="8"/>
       <c r="K28" s="8"/>
@@ -1883,10 +1874,10 @@
         <v>32</v>
       </c>
       <c r="B29" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C29" s="8" t="s">
         <v>22</v>
-      </c>
-      <c r="C29" s="12" t="s">
-        <v>73</v>
       </c>
       <c r="D29" s="8"/>
       <c r="E29" s="8"/>
@@ -1898,7 +1889,7 @@
         <v>25</v>
       </c>
       <c r="I29" s="9" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="J29" s="8"/>
       <c r="K29" s="8"/>
@@ -1915,10 +1906,10 @@
         <v>32</v>
       </c>
       <c r="B30" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C30" s="8" t="s">
         <v>22</v>
-      </c>
-      <c r="C30" s="12" t="s">
-        <v>74</v>
       </c>
       <c r="D30" s="8"/>
       <c r="E30" s="8"/>
@@ -1930,7 +1921,7 @@
         <v>25</v>
       </c>
       <c r="I30" s="9" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="J30" s="8"/>
       <c r="K30" s="8"/>
@@ -1947,10 +1938,10 @@
         <v>32</v>
       </c>
       <c r="B31" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C31" s="8" t="s">
         <v>22</v>
-      </c>
-      <c r="C31" s="12" t="s">
-        <v>76</v>
       </c>
       <c r="D31" s="8"/>
       <c r="E31" s="8"/>
@@ -1962,7 +1953,7 @@
         <v>25</v>
       </c>
       <c r="I31" s="9" t="s">
-        <v>86</v>
+        <v>66</v>
       </c>
       <c r="J31" s="8"/>
       <c r="K31" s="8"/>
@@ -1979,10 +1970,10 @@
         <v>32</v>
       </c>
       <c r="B32" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C32" s="8" t="s">
         <v>22</v>
-      </c>
-      <c r="C32" s="12" t="s">
-        <v>77</v>
       </c>
       <c r="D32" s="8"/>
       <c r="E32" s="8"/>
@@ -1994,7 +1985,7 @@
         <v>25</v>
       </c>
       <c r="I32" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J32" s="8"/>
       <c r="K32" s="8"/>
@@ -2011,10 +2002,10 @@
         <v>32</v>
       </c>
       <c r="B33" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C33" s="8" t="s">
         <v>22</v>
-      </c>
-      <c r="C33" s="12" t="s">
-        <v>71</v>
       </c>
       <c r="D33" s="8"/>
       <c r="E33" s="8"/>
@@ -2026,7 +2017,7 @@
         <v>25</v>
       </c>
       <c r="I33" s="9" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
       <c r="J33" s="8"/>
       <c r="K33" s="8"/>
@@ -2043,10 +2034,10 @@
         <v>32</v>
       </c>
       <c r="B34" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C34" s="8" t="s">
         <v>22</v>
-      </c>
-      <c r="C34" s="12" t="s">
-        <v>72</v>
       </c>
       <c r="D34" s="8"/>
       <c r="E34" s="8"/>
@@ -2075,10 +2066,10 @@
         <v>32</v>
       </c>
       <c r="B35" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="C35" s="8" t="s">
         <v>22</v>
-      </c>
-      <c r="C35" s="12" t="s">
-        <v>88</v>
       </c>
       <c r="D35" s="8"/>
       <c r="E35" s="8"/>
@@ -2090,7 +2081,7 @@
         <v>25</v>
       </c>
       <c r="I35" s="9" t="s">
-        <v>89</v>
+        <v>68</v>
       </c>
       <c r="J35" s="8"/>
       <c r="K35" s="8"/>
@@ -2107,10 +2098,10 @@
         <v>32</v>
       </c>
       <c r="B36" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C36" s="8" t="s">
         <v>22</v>
-      </c>
-      <c r="C36" s="12" t="s">
-        <v>33</v>
       </c>
       <c r="D36" s="8"/>
       <c r="E36" s="8"/>
@@ -2122,7 +2113,7 @@
         <v>25</v>
       </c>
       <c r="I36" s="9" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="J36" s="8"/>
       <c r="K36" s="8"/>
@@ -2139,10 +2130,10 @@
         <v>32</v>
       </c>
       <c r="B37" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="C37" s="8" t="s">
         <v>16</v>
-      </c>
-      <c r="C37" s="12" t="s">
-        <v>90</v>
       </c>
       <c r="D37" s="8"/>
       <c r="E37" s="8"/>
@@ -2154,7 +2145,7 @@
         <v>25</v>
       </c>
       <c r="I37" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J37" s="8"/>
       <c r="K37" s="8"/>
@@ -2171,10 +2162,10 @@
         <v>32</v>
       </c>
       <c r="B38" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="C38" s="8" t="s">
         <v>16</v>
-      </c>
-      <c r="C38" s="12" t="s">
-        <v>91</v>
       </c>
       <c r="D38" s="8"/>
       <c r="E38" s="8"/>
@@ -2186,7 +2177,7 @@
         <v>25</v>
       </c>
       <c r="I38" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J38" s="8"/>
       <c r="K38" s="8"/>
@@ -2203,10 +2194,10 @@
         <v>32</v>
       </c>
       <c r="B39" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C39" s="8" t="s">
         <v>16</v>
-      </c>
-      <c r="C39" s="12" t="s">
-        <v>92</v>
       </c>
       <c r="D39" s="8"/>
       <c r="E39" s="8"/>
@@ -2235,10 +2226,10 @@
         <v>32</v>
       </c>
       <c r="B40" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C40" s="8" t="s">
         <v>16</v>
-      </c>
-      <c r="C40" s="12" t="s">
-        <v>93</v>
       </c>
       <c r="D40" s="8"/>
       <c r="E40" s="8"/>
@@ -2250,7 +2241,7 @@
         <v>25</v>
       </c>
       <c r="I40" s="9" t="s">
-        <v>94</v>
+        <v>69</v>
       </c>
       <c r="J40" s="8"/>
       <c r="K40" s="8"/>
@@ -2267,10 +2258,10 @@
         <v>32</v>
       </c>
       <c r="B41" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="C41" s="8" t="s">
         <v>22</v>
-      </c>
-      <c r="C41" s="12" t="s">
-        <v>95</v>
       </c>
       <c r="D41" s="8"/>
       <c r="E41" s="8"/>
@@ -2282,7 +2273,7 @@
         <v>25</v>
       </c>
       <c r="I41" s="9" t="s">
-        <v>96</v>
+        <v>70</v>
       </c>
       <c r="J41" s="8"/>
       <c r="K41" s="8"/>
@@ -2299,10 +2290,10 @@
         <v>32</v>
       </c>
       <c r="B42" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="C42" s="8" t="s">
         <v>22</v>
-      </c>
-      <c r="C42" s="12" t="s">
-        <v>97</v>
       </c>
       <c r="D42" s="8"/>
       <c r="E42" s="8"/>
@@ -2314,7 +2305,7 @@
         <v>25</v>
       </c>
       <c r="I42" s="9" t="s">
-        <v>96</v>
+        <v>70</v>
       </c>
       <c r="J42" s="8"/>
       <c r="K42" s="8"/>
@@ -2331,10 +2322,10 @@
         <v>32</v>
       </c>
       <c r="B43" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="C43" s="8" t="s">
         <v>22</v>
-      </c>
-      <c r="C43" s="12" t="s">
-        <v>98</v>
       </c>
       <c r="D43" s="8"/>
       <c r="E43" s="8"/>
@@ -2346,7 +2337,7 @@
         <v>25</v>
       </c>
       <c r="I43" s="9" t="s">
-        <v>96</v>
+        <v>70</v>
       </c>
       <c r="J43" s="8"/>
       <c r="K43" s="8"/>
@@ -2363,10 +2354,10 @@
         <v>32</v>
       </c>
       <c r="B44" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="C44" s="8" t="s">
         <v>22</v>
-      </c>
-      <c r="C44" s="12" t="s">
-        <v>99</v>
       </c>
       <c r="D44" s="8"/>
       <c r="E44" s="8"/>
@@ -2378,7 +2369,7 @@
         <v>25</v>
       </c>
       <c r="I44" s="9" t="s">
-        <v>100</v>
+        <v>71</v>
       </c>
       <c r="J44" s="8"/>
       <c r="K44" s="8"/>
@@ -2395,16 +2386,16 @@
         <v>32</v>
       </c>
       <c r="B45" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="C45" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C45" s="12" t="s">
-        <v>102</v>
-      </c>
       <c r="D45" s="8" t="s">
-        <v>101</v>
+        <v>72</v>
       </c>
       <c r="E45" s="8" t="s">
-        <v>101</v>
+        <v>72</v>
       </c>
       <c r="F45" s="8"/>
       <c r="G45" s="12" t="s">
@@ -2415,13 +2406,13 @@
       </c>
       <c r="I45" s="9"/>
       <c r="J45" s="8" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="K45" s="8" t="s">
         <v>31</v>
       </c>
       <c r="L45" s="8" t="s">
-        <v>103</v>
+        <v>73</v>
       </c>
       <c r="M45" s="8"/>
       <c r="N45" s="8"/>
@@ -2435,10 +2426,10 @@
         <v>32</v>
       </c>
       <c r="B46" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C46" s="12" t="s">
         <v>22</v>
-      </c>
-      <c r="C46" s="12" t="s">
-        <v>48</v>
       </c>
       <c r="D46" s="8" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
working implementation of PrOD RASs.
</commit_message>
<xml_diff>
--- a/tabular/contributed/190612 DSV TABLE.xlsx
+++ b/tabular/contributed/190612 DSV TABLE.xlsx
@@ -9,11 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6820" yWindow="460" windowWidth="43020" windowHeight="26380"/>
+    <workbookView xWindow="1940" yWindow="1700" windowWidth="43360" windowHeight="26380"/>
   </bookViews>
   <sheets>
     <sheet name="DSV" sheetId="3" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DSV!$A$1:$P$45</definedName>
+  </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -30,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="97">
   <si>
     <t>gene</t>
   </si>
@@ -56,9 +59,6 @@
     <t>vitroOrVivo</t>
   </si>
   <si>
-    <t>ec50 fold change</t>
-  </si>
-  <si>
     <t>clinicalTrialName</t>
   </si>
   <si>
@@ -125,18 +125,9 @@
     <t>DSV</t>
   </si>
   <si>
-    <t>PrOD</t>
-  </si>
-  <si>
     <t>NS5B</t>
   </si>
   <si>
-    <t>PEARL III, IV</t>
-  </si>
-  <si>
-    <t>PrOD+/-RBV</t>
-  </si>
-  <si>
     <t>10</t>
   </si>
   <si>
@@ -164,39 +155,15 @@
     <t>TN &amp; TE; noncirrhotic and cirrhotic</t>
   </si>
   <si>
-    <t>PrOD +/- RBV</t>
-  </si>
-  <si>
-    <t>PrOD+RBV</t>
-  </si>
-  <si>
-    <t>Turquoise II</t>
-  </si>
-  <si>
-    <t>Sapphire II, Turquoise II, Pearl IV</t>
-  </si>
-  <si>
     <t>Pooled</t>
   </si>
   <si>
-    <t>Sarrazin, EASL Paris, 23-24 Sep, 2016</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sapphire II </t>
-  </si>
-  <si>
     <t>TE, non cirrhotic</t>
   </si>
   <si>
-    <t>Turquoise I</t>
-  </si>
-  <si>
     <t xml:space="preserve">TE, cirrhotic </t>
   </si>
   <si>
-    <t>real world, retrospective</t>
-  </si>
-  <si>
     <t>2-20</t>
   </si>
   <si>
@@ -248,12 +215,6 @@
     <t>2.4</t>
   </si>
   <si>
-    <t>NK</t>
-  </si>
-  <si>
-    <t>cirrhosis</t>
-  </si>
-  <si>
     <t>556G</t>
   </si>
   <si>
@@ -332,7 +293,37 @@
     <t>495A</t>
   </si>
   <si>
-    <t>316Y+414I</t>
+    <t>Pooled1</t>
+  </si>
+  <si>
+    <t>Pooled2</t>
+  </si>
+  <si>
+    <t>SAPPHIRE-II</t>
+  </si>
+  <si>
+    <t>Case report*</t>
+  </si>
+  <si>
+    <t>TURQUOISE-I</t>
+  </si>
+  <si>
+    <t>Retrospective real world study*</t>
+  </si>
+  <si>
+    <t>PTV_r_OBV_DSV</t>
+  </si>
+  <si>
+    <t>PTV_r_OBV_DSV;PTV_r_OBV_DSV_RBV</t>
+  </si>
+  <si>
+    <t>PTV_r_OBV_DSV_RBV</t>
+  </si>
+  <si>
+    <t>EASL_2016_Abs_LBP503</t>
+  </si>
+  <si>
+    <t>ec50</t>
   </si>
 </sst>
 </file>
@@ -758,12 +749,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P46"/>
+  <dimension ref="A1:P45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="168" zoomScaleNormal="168" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="I1" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1:B1048576"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -811,66 +802,68 @@
         <v>7</v>
       </c>
       <c r="I1" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="J1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="N1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="O1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="7" t="s">
         <v>14</v>
-      </c>
-      <c r="P1" s="7" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>23</v>
-      </c>
       <c r="I2" s="9"/>
-      <c r="J2" s="2"/>
+      <c r="J2" s="2" t="s">
+        <v>89</v>
+      </c>
       <c r="K2" s="8" t="s">
-        <v>31</v>
+        <v>92</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M2" s="8"/>
       <c r="N2" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O2" s="11">
         <v>29575060</v>
@@ -879,40 +872,42 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="C3" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>23</v>
-      </c>
       <c r="I3" s="9"/>
-      <c r="J3" s="2"/>
+      <c r="J3" s="2" t="s">
+        <v>89</v>
+      </c>
       <c r="K3" s="8" t="s">
-        <v>31</v>
+        <v>92</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M3" s="8"/>
       <c r="N3" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O3" s="11">
         <v>29575060</v>
@@ -921,38 +916,38 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="C4" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>17</v>
-      </c>
       <c r="F4" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I4" s="9"/>
       <c r="J4" s="8" t="s">
-        <v>33</v>
+        <v>86</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>34</v>
+        <v>93</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M4" s="8"/>
       <c r="N4" s="2"/>
@@ -963,38 +958,38 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="C5" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="8" t="s">
-        <v>17</v>
-      </c>
       <c r="E5" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I5" s="9"/>
       <c r="J5" s="8" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="K5" s="8" t="s">
-        <v>34</v>
+        <v>93</v>
       </c>
       <c r="L5" s="8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="M5" s="8"/>
       <c r="N5" s="2"/>
@@ -1005,38 +1000,38 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="C6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="F6" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>19</v>
-      </c>
       <c r="G6" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I6" s="9"/>
       <c r="J6" s="8" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="K6" s="8" t="s">
-        <v>34</v>
+        <v>93</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="M6" s="8"/>
       <c r="N6" s="2"/>
@@ -1047,38 +1042,38 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="C7" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="E7" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="8" t="s">
-        <v>18</v>
-      </c>
       <c r="F7" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I7" s="9"/>
       <c r="J7" s="8" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="K7" s="8" t="s">
-        <v>34</v>
+        <v>93</v>
       </c>
       <c r="L7" s="8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="M7" s="8"/>
       <c r="N7" s="2"/>
@@ -1089,38 +1084,38 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="C8" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="F8" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>19</v>
-      </c>
       <c r="G8" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I8" s="9"/>
       <c r="J8" s="8" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="K8" s="8" t="s">
-        <v>34</v>
+        <v>93</v>
       </c>
       <c r="L8" s="8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="M8" s="8"/>
       <c r="N8" s="2"/>
@@ -1131,38 +1126,38 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="C9" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="F9" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>19</v>
-      </c>
       <c r="G9" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I9" s="9"/>
       <c r="J9" s="8" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="K9" s="8" t="s">
-        <v>34</v>
+        <v>93</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="M9" s="8"/>
       <c r="N9" s="2"/>
@@ -1173,38 +1168,38 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="C10" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="F10" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>19</v>
-      </c>
       <c r="G10" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I10" s="9"/>
       <c r="J10" s="8" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="K10" s="8" t="s">
-        <v>34</v>
+        <v>93</v>
       </c>
       <c r="L10" s="8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="M10" s="8"/>
       <c r="N10" s="2"/>
@@ -1215,38 +1210,38 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="C11" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="E11" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="8" t="s">
-        <v>18</v>
-      </c>
       <c r="F11" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I11" s="9"/>
       <c r="J11" s="8" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="K11" s="8" t="s">
-        <v>34</v>
+        <v>93</v>
       </c>
       <c r="L11" s="8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="M11" s="8"/>
       <c r="N11" s="2"/>
@@ -1257,38 +1252,38 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C12" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>17</v>
-      </c>
       <c r="F12" s="8" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I12" s="9"/>
       <c r="J12" s="8" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="K12" s="8" t="s">
-        <v>34</v>
+        <v>93</v>
       </c>
       <c r="L12" s="8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="M12" s="8"/>
       <c r="N12" s="2"/>
@@ -1299,38 +1294,38 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="C13" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H13" s="8" t="s">
         <v>22</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="G13" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="H13" s="8" t="s">
-        <v>23</v>
       </c>
       <c r="I13" s="9"/>
       <c r="J13" s="8" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="K13" s="8" t="s">
-        <v>31</v>
+        <v>92</v>
       </c>
       <c r="L13" s="8" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="M13" s="8"/>
       <c r="N13" s="2"/>
@@ -1341,80 +1336,80 @@
     </row>
     <row r="14" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="C14" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="E14" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E14" s="8" t="s">
-        <v>18</v>
-      </c>
       <c r="F14" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I14" s="9"/>
       <c r="J14" s="8" t="s">
-        <v>47</v>
+        <v>87</v>
       </c>
       <c r="K14" s="9" t="s">
-        <v>44</v>
+        <v>93</v>
       </c>
       <c r="L14" s="8" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="M14" s="8"/>
       <c r="N14" s="8" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="O14" s="8" t="s">
-        <v>49</v>
+        <v>95</v>
       </c>
       <c r="P14" s="8"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="C15" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="12" t="s">
         <v>16</v>
-      </c>
-      <c r="D15" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="E15" s="12" t="s">
-        <v>17</v>
       </c>
       <c r="F15" s="8"/>
       <c r="G15" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I15" s="9"/>
       <c r="J15" s="12" t="s">
-        <v>50</v>
+        <v>88</v>
       </c>
       <c r="K15" s="8" t="s">
-        <v>45</v>
+        <v>94</v>
       </c>
       <c r="L15" s="8" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="M15" s="2"/>
       <c r="N15" s="8"/>
@@ -1425,36 +1420,36 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F16" s="8"/>
       <c r="G16" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I16" s="9"/>
       <c r="J16" s="12" t="s">
-        <v>50</v>
+        <v>88</v>
       </c>
       <c r="K16" s="8" t="s">
-        <v>45</v>
+        <v>94</v>
       </c>
       <c r="L16" s="8" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="M16" s="2"/>
       <c r="N16" s="8"/>
@@ -1465,36 +1460,36 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="C17" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="8" t="s">
         <v>16</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>17</v>
       </c>
       <c r="F17" s="8"/>
       <c r="G17" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H17" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I17" s="9"/>
       <c r="J17" s="8" t="s">
-        <v>52</v>
+        <v>90</v>
       </c>
       <c r="K17" s="8" t="s">
-        <v>45</v>
+        <v>94</v>
       </c>
       <c r="L17" s="8" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="M17" s="2"/>
       <c r="N17" s="8"/>
@@ -1505,33 +1500,33 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="C18" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" s="12" t="s">
         <v>16</v>
-      </c>
-      <c r="D18" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="E18" s="12" t="s">
-        <v>17</v>
       </c>
       <c r="F18" s="8"/>
       <c r="G18" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H18" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I18" s="9"/>
       <c r="J18" s="8" t="s">
-        <v>54</v>
+        <v>91</v>
       </c>
       <c r="K18" s="8" t="s">
-        <v>31</v>
+        <v>92</v>
       </c>
       <c r="L18" s="8"/>
       <c r="M18" s="8"/>
@@ -1543,30 +1538,34 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F19" s="8"/>
       <c r="G19" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H19" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I19" s="9"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="8"/>
+      <c r="J19" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="K19" s="8" t="s">
+        <v>92</v>
+      </c>
       <c r="L19" s="8"/>
       <c r="M19" s="8"/>
       <c r="N19" s="8"/>
@@ -1577,25 +1576,25 @@
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
       <c r="G20" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I20" s="9" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="J20" s="8"/>
       <c r="K20" s="8"/>
@@ -1609,25 +1608,25 @@
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
       <c r="G21" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H21" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I21" s="9" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="J21" s="8"/>
       <c r="K21" s="8"/>
@@ -1641,33 +1640,33 @@
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F22" s="8"/>
       <c r="G22" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H22" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I22" s="9"/>
       <c r="J22" s="8" t="s">
-        <v>54</v>
+        <v>91</v>
       </c>
       <c r="K22" s="8" t="s">
-        <v>31</v>
+        <v>92</v>
       </c>
       <c r="L22" s="8"/>
       <c r="M22" s="8"/>
@@ -1679,25 +1678,25 @@
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D23" s="8"/>
       <c r="E23" s="8"/>
       <c r="F23" s="8"/>
       <c r="G23" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I23" s="9" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="J23" s="8"/>
       <c r="K23" s="8"/>
@@ -1711,25 +1710,25 @@
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D24" s="8"/>
       <c r="E24" s="8"/>
       <c r="F24" s="8"/>
       <c r="G24" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H24" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I24" s="9" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="J24" s="8"/>
       <c r="K24" s="8"/>
@@ -1743,25 +1742,25 @@
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D25" s="8"/>
       <c r="E25" s="8"/>
       <c r="F25" s="8"/>
       <c r="G25" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H25" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I25" s="9" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="J25" s="8"/>
       <c r="K25" s="8"/>
@@ -1775,25 +1774,25 @@
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D26" s="8"/>
       <c r="E26" s="8"/>
       <c r="F26" s="8"/>
       <c r="G26" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H26" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I26" s="9" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="J26" s="8"/>
       <c r="K26" s="8"/>
@@ -1807,25 +1806,25 @@
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D27" s="8"/>
       <c r="E27" s="8"/>
       <c r="F27" s="8"/>
       <c r="G27" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H27" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I27" s="9" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="J27" s="8"/>
       <c r="K27" s="8"/>
@@ -1839,25 +1838,25 @@
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D28" s="8"/>
       <c r="E28" s="8"/>
       <c r="F28" s="8"/>
       <c r="G28" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H28" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I28" s="9" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="J28" s="8"/>
       <c r="K28" s="8"/>
@@ -1871,25 +1870,25 @@
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D29" s="8"/>
       <c r="E29" s="8"/>
       <c r="F29" s="8"/>
       <c r="G29" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H29" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I29" s="9" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="J29" s="8"/>
       <c r="K29" s="8"/>
@@ -1903,25 +1902,25 @@
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D30" s="8"/>
       <c r="E30" s="8"/>
       <c r="F30" s="8"/>
       <c r="G30" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H30" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I30" s="9" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="J30" s="8"/>
       <c r="K30" s="8"/>
@@ -1935,25 +1934,25 @@
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D31" s="8"/>
       <c r="E31" s="8"/>
       <c r="F31" s="8"/>
       <c r="G31" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H31" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I31" s="9" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="J31" s="8"/>
       <c r="K31" s="8"/>
@@ -1967,25 +1966,25 @@
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D32" s="8"/>
       <c r="E32" s="8"/>
       <c r="F32" s="8"/>
       <c r="G32" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H32" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I32" s="9" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="J32" s="8"/>
       <c r="K32" s="8"/>
@@ -1999,25 +1998,25 @@
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A33" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D33" s="8"/>
       <c r="E33" s="8"/>
       <c r="F33" s="8"/>
       <c r="G33" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H33" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I33" s="9" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="J33" s="8"/>
       <c r="K33" s="8"/>
@@ -2031,25 +2030,25 @@
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A34" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D34" s="8"/>
       <c r="E34" s="8"/>
       <c r="F34" s="8"/>
       <c r="G34" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H34" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I34" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J34" s="8"/>
       <c r="K34" s="8"/>
@@ -2063,25 +2062,25 @@
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A35" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D35" s="8"/>
       <c r="E35" s="8"/>
       <c r="F35" s="8"/>
       <c r="G35" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H35" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I35" s="9" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="J35" s="8"/>
       <c r="K35" s="8"/>
@@ -2095,25 +2094,25 @@
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A36" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D36" s="8"/>
       <c r="E36" s="8"/>
       <c r="F36" s="8"/>
       <c r="G36" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H36" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I36" s="9" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="J36" s="8"/>
       <c r="K36" s="8"/>
@@ -2127,25 +2126,25 @@
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A37" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D37" s="8"/>
       <c r="E37" s="8"/>
       <c r="F37" s="8"/>
       <c r="G37" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H37" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I37" s="9" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="J37" s="8"/>
       <c r="K37" s="8"/>
@@ -2159,25 +2158,25 @@
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A38" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D38" s="8"/>
       <c r="E38" s="8"/>
       <c r="F38" s="8"/>
       <c r="G38" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H38" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I38" s="9" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="J38" s="8"/>
       <c r="K38" s="8"/>
@@ -2191,25 +2190,25 @@
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A39" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D39" s="8"/>
       <c r="E39" s="8"/>
       <c r="F39" s="8"/>
       <c r="G39" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H39" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="I39" s="9" t="s">
         <v>25</v>
-      </c>
-      <c r="I39" s="9" t="s">
-        <v>26</v>
       </c>
       <c r="J39" s="8"/>
       <c r="K39" s="8"/>
@@ -2223,25 +2222,25 @@
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A40" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D40" s="8"/>
       <c r="E40" s="8"/>
       <c r="F40" s="8"/>
       <c r="G40" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H40" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I40" s="9" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="J40" s="8"/>
       <c r="K40" s="8"/>
@@ -2255,25 +2254,25 @@
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A41" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D41" s="8"/>
       <c r="E41" s="8"/>
       <c r="F41" s="8"/>
       <c r="G41" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H41" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I41" s="9" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="J41" s="8"/>
       <c r="K41" s="8"/>
@@ -2287,25 +2286,25 @@
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A42" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D42" s="8"/>
       <c r="E42" s="8"/>
       <c r="F42" s="8"/>
       <c r="G42" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H42" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I42" s="9" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="J42" s="8"/>
       <c r="K42" s="8"/>
@@ -2319,25 +2318,25 @@
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A43" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D43" s="8"/>
       <c r="E43" s="8"/>
       <c r="F43" s="8"/>
       <c r="G43" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H43" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I43" s="9" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="J43" s="8"/>
       <c r="K43" s="8"/>
@@ -2351,25 +2350,25 @@
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A44" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D44" s="8"/>
       <c r="E44" s="8"/>
       <c r="F44" s="8"/>
       <c r="G44" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H44" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I44" s="9" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="J44" s="8"/>
       <c r="K44" s="8"/>
@@ -2383,83 +2382,46 @@
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A45" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B45" s="12" t="s">
-        <v>100</v>
+        <v>68</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>72</v>
+        <v>16</v>
       </c>
       <c r="E45" s="8" t="s">
-        <v>72</v>
+        <v>16</v>
       </c>
       <c r="F45" s="8"/>
       <c r="G45" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H45" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I45" s="9"/>
       <c r="J45" s="8" t="s">
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="K45" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="L45" s="8" t="s">
-        <v>73</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="L45" s="8"/>
       <c r="M45" s="8"/>
-      <c r="N45" s="8"/>
+      <c r="N45" s="8" t="s">
+        <v>23</v>
+      </c>
       <c r="O45" s="8">
-        <v>24725237</v>
+        <v>27670383</v>
       </c>
       <c r="P45" s="8"/>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A46" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="B46" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="C46" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D46" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E46" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="F46" s="8"/>
-      <c r="G46" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="H46" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="I46" s="9"/>
-      <c r="J46" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="K46" s="8"/>
-      <c r="L46" s="8"/>
-      <c r="M46" s="8"/>
-      <c r="N46" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="O46" s="8">
-        <v>27670383</v>
-      </c>
-      <c r="P46" s="8"/>
-    </row>
   </sheetData>
+  <autoFilter ref="A1:P45"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>